<commit_message>
added figures and tables to word doc
</commit_message>
<xml_diff>
--- a/src/Grid_Independence_Test.xlsx
+++ b/src/Grid_Independence_Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grobl\Documents\Project\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F3BC9E-7F4F-45C8-933A-96B9D6DF2F46}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F5C723-E637-4B95-9BC9-FB1FCE1695E6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" xr2:uid="{95A8A740-73A1-4569-8FB2-8A4DD4344269}"/>
   </bookViews>
@@ -66,12 +66,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -80,10 +95,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -403,7 +418,7 @@
   <dimension ref="C4:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,119 +431,119 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C6" s="1">
+      <c r="C6" s="2">
         <v>20</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2">
         <v>456</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1">
+      <c r="F6" s="2"/>
+      <c r="G6" s="2">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="1">
+      <c r="C7" s="2">
         <v>50</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2">
         <v>2572</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1">
+      <c r="F7" s="2"/>
+      <c r="G7" s="2">
         <v>90</v>
       </c>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <v>100</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2">
         <v>9093</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1">
+      <c r="F8" s="2"/>
+      <c r="G8" s="2">
         <v>365</v>
       </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="1">
+      <c r="C9" s="2">
         <v>150</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2">
         <v>18750</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1">
+      <c r="F9" s="2"/>
+      <c r="G9" s="2">
         <v>825</v>
       </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="1">
+      <c r="C10" s="2">
         <v>200</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2">
         <v>31115</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1">
+      <c r="F10" s="2"/>
+      <c r="G10" s="2">
         <v>1470</v>
       </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="1">
+      <c r="C11" s="2">
         <v>250</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2">
         <v>45890</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1">
+      <c r="F11" s="2"/>
+      <c r="G11" s="2">
         <v>2302</v>
       </c>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="1">
+      <c r="C12" s="2">
         <v>300</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2">
         <v>62848</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1">
+      <c r="F12" s="2"/>
+      <c r="G12" s="2">
         <v>3318</v>
       </c>
     </row>

</xml_diff>